<commit_message>
Fix: Read 'All' sheet from Excel file
</commit_message>
<xml_diff>
--- a/backend/data/rudraram_survey.xlsx
+++ b/backend/data/rudraram_survey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iiithydresearch-my.sharepoint.com/personal/ritik_yelekar_research_iiit_ac_in/Documents/Startup/EvaraTech/Projects/TTDF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\OneDrive\Desktop\StartUp\Rudraram Survey\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9045FA8B-AB01-4323-BF2C-5B66BBBD3005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9D1656-233A-4985-8024-B25F07D41354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -718,7 +718,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -730,16 +730,19 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -942,19 +945,19 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1187,16 +1190,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="39.140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="39.140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="16.140625" customWidth="1"/>
@@ -1212,7 +1215,7 @@
     <col min="12" max="12" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.15">
+    <row r="1" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1253,23 +1256,23 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" hidden="1" customHeight="1">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="17"/>
-    </row>
-    <row r="3" spans="1:13" ht="13.15" hidden="1">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="14"/>
+    </row>
+    <row r="3" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -1297,7 +1300,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="13.15" hidden="1">
+    <row r="4" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1325,7 +1328,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="13.15">
+    <row r="5" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -1353,7 +1356,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="13.15">
+    <row r="6" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
@@ -1381,7 +1384,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="13.15" hidden="1">
+    <row r="7" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -1409,7 +1412,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="13.15" hidden="1">
+    <row r="8" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
@@ -1437,7 +1440,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="13.15" hidden="1">
+    <row r="9" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
@@ -1465,7 +1468,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="13.15" hidden="1">
+    <row r="10" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>45</v>
       </c>
@@ -1493,7 +1496,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="13.15" hidden="1">
+    <row r="11" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
@@ -1521,7 +1524,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="13.15" hidden="1">
+    <row r="12" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -1549,7 +1552,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="13.15" hidden="1">
+    <row r="13" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>53</v>
       </c>
@@ -1577,7 +1580,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="13.15" hidden="1">
+    <row r="14" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>56</v>
       </c>
@@ -1605,7 +1608,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="13.15" hidden="1">
+    <row r="15" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>58</v>
       </c>
@@ -1633,7 +1636,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="13.15" hidden="1">
+    <row r="16" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>59</v>
       </c>
@@ -1661,7 +1664,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="13.15" hidden="1">
+    <row r="17" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>62</v>
       </c>
@@ -1689,7 +1692,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="13.15">
+    <row r="18" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>64</v>
       </c>
@@ -1717,7 +1720,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="13.15">
+    <row r="19" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>65</v>
       </c>
@@ -1745,23 +1748,23 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" hidden="1" customHeight="1">
-      <c r="A20" s="18" t="s">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="17"/>
-    </row>
-    <row r="21" spans="1:12" ht="13.15" hidden="1">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="14"/>
+    </row>
+    <row r="21" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>68</v>
       </c>
@@ -1789,7 +1792,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="13.15" hidden="1">
+    <row r="22" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>72</v>
       </c>
@@ -1817,7 +1820,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="13.15" hidden="1">
+    <row r="23" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>74</v>
       </c>
@@ -1845,7 +1848,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="13.15" hidden="1">
+    <row r="24" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>77</v>
       </c>
@@ -1873,7 +1876,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="13.15" hidden="1">
+    <row r="25" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>79</v>
       </c>
@@ -1901,7 +1904,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="13.15" hidden="1">
+    <row r="26" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>81</v>
       </c>
@@ -1929,7 +1932,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="13.15" hidden="1">
+    <row r="27" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>83</v>
       </c>
@@ -1957,7 +1960,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="13.15" hidden="1">
+    <row r="28" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>85</v>
       </c>
@@ -1985,7 +1988,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="13.15" hidden="1">
+    <row r="29" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>88</v>
       </c>
@@ -2013,7 +2016,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="13.15" hidden="1">
+    <row r="30" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>90</v>
       </c>
@@ -2041,7 +2044,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="13.15" hidden="1">
+    <row r="31" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>93</v>
       </c>
@@ -2069,7 +2072,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="13.15" hidden="1">
+    <row r="32" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>95</v>
       </c>
@@ -2097,7 +2100,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="13.15" hidden="1">
+    <row r="33" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>96</v>
       </c>
@@ -2125,23 +2128,23 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" hidden="1" customHeight="1">
-      <c r="A34" s="18" t="s">
+    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="17"/>
-    </row>
-    <row r="35" spans="1:12" ht="13.15" hidden="1">
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="14"/>
+    </row>
+    <row r="35" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>100</v>
       </c>
@@ -2169,7 +2172,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="13.15" hidden="1">
+    <row r="36" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>103</v>
       </c>
@@ -2197,7 +2200,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="13.15" hidden="1">
+    <row r="37" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>104</v>
       </c>
@@ -2225,7 +2228,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="13.15" hidden="1">
+    <row r="38" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>107</v>
       </c>
@@ -2253,7 +2256,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="13.15">
+    <row r="39" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>110</v>
       </c>
@@ -2281,7 +2284,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="13.15">
+    <row r="40" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>111</v>
       </c>
@@ -2309,7 +2312,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="13.15" hidden="1">
+    <row r="41" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>113</v>
       </c>
@@ -2337,7 +2340,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="13.15" hidden="1">
+    <row r="42" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>115</v>
       </c>
@@ -2365,7 +2368,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="13.15" hidden="1">
+    <row r="43" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>117</v>
       </c>
@@ -2393,7 +2396,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="13.15" hidden="1">
+    <row r="44" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>120</v>
       </c>
@@ -2421,7 +2424,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="13.15" hidden="1">
+    <row r="45" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>124</v>
       </c>
@@ -2449,7 +2452,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="13.15" hidden="1">
+    <row r="46" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>127</v>
       </c>
@@ -2477,7 +2480,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="13.15" hidden="1">
+    <row r="47" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>130</v>
       </c>
@@ -2505,7 +2508,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="13.15" hidden="1">
+    <row r="48" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>132</v>
       </c>
@@ -2533,7 +2536,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="13.15" hidden="1">
+    <row r="49" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>135</v>
       </c>
@@ -2561,7 +2564,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="13.15" hidden="1">
+    <row r="50" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>137</v>
       </c>
@@ -2589,7 +2592,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="13.15" hidden="1">
+    <row r="51" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>140</v>
       </c>
@@ -2617,7 +2620,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="13.15" hidden="1">
+    <row r="52" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>143</v>
       </c>
@@ -2645,7 +2648,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="13.15" hidden="1">
+    <row r="53" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>147</v>
       </c>
@@ -2673,7 +2676,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="13.15" hidden="1">
+    <row r="54" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>150</v>
       </c>
@@ -2701,7 +2704,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="13.15" hidden="1">
+    <row r="55" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>154</v>
       </c>
@@ -2729,7 +2732,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="13.15" hidden="1">
+    <row r="56" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>157</v>
       </c>
@@ -2757,7 +2760,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="13.15" hidden="1">
+    <row r="57" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>159</v>
       </c>
@@ -2785,7 +2788,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="13.15" hidden="1">
+    <row r="58" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>160</v>
       </c>
@@ -2813,7 +2816,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="13.15" hidden="1">
+    <row r="59" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>162</v>
       </c>
@@ -2841,7 +2844,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="13.15" hidden="1">
+    <row r="60" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>165</v>
       </c>
@@ -2869,7 +2872,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="13.15" hidden="1">
+    <row r="61" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>168</v>
       </c>
@@ -2897,7 +2900,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="13.15" hidden="1">
+    <row r="62" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>171</v>
       </c>
@@ -2925,7 +2928,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="13.15">
+    <row r="63" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>173</v>
       </c>
@@ -2953,7 +2956,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="13.15">
+    <row r="64" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>176</v>
       </c>
@@ -2982,14 +2985,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M64" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="OHT"/>
-        <filter val="Sump"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:M64" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="3">
     <mergeCell ref="A20:L20"/>
     <mergeCell ref="A2:L2"/>
@@ -3004,11 +3000,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.5703125" defaultRowHeight="21.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="22.5703125" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
@@ -3024,7 +3020,7 @@
     <col min="13" max="13" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21.75" customHeight="1">
+    <row r="1" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>178</v>
       </c>
@@ -3071,7 +3067,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="2" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3104,7 +3100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="3" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3136,7 +3132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="4" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3168,7 +3164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="5" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3200,7 +3196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="6" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3232,7 +3228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="7" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3264,7 +3260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="8" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3296,7 +3292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="9" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3328,7 +3324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="10" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3360,7 +3356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="11" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3392,7 +3388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="12" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3424,7 +3420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="13" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3456,7 +3452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="14" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3488,7 +3484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="15" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3520,7 +3516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="16" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3552,7 +3548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="17" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3584,7 +3580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="18" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3616,7 +3612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="19" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3648,7 +3644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="20" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3680,7 +3676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="21" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3712,7 +3708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="22" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3744,7 +3740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="23" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3776,7 +3772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="24" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3808,7 +3804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="25" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3840,7 +3836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="26" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3872,7 +3868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="27" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3904,7 +3900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="21.75" customHeight="1">
+    <row r="28" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3938,7 +3934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="21.75" customHeight="1">
+    <row r="29" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3970,7 +3966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="30" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4002,7 +3998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="31" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4034,7 +4030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="21.75" customHeight="1">
+    <row r="32" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4066,7 +4062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="21.75" customHeight="1">
+    <row r="33" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4098,7 +4094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="21.75" customHeight="1">
+    <row r="34" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4130,7 +4126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="35" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4162,7 +4158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="36" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4194,7 +4190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="37" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4226,7 +4222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="21.75" customHeight="1">
+    <row r="38" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4258,7 +4254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="39" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4290,7 +4286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="40" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4322,7 +4318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="21.75" customHeight="1">
+    <row r="41" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4354,7 +4350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="21.75" customHeight="1">
+    <row r="42" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4386,7 +4382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="43" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4418,7 +4414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="44" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4450,7 +4446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="45" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4482,7 +4478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="46" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4514,7 +4510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="47" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4546,7 +4542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="48" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4578,7 +4574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="49" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4610,7 +4606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="50" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4642,7 +4638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="21.75" customHeight="1">
+    <row r="51" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4674,7 +4670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="21.75" customHeight="1">
+    <row r="52" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4706,7 +4702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="21.75" customHeight="1">
+    <row r="53" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4764,7 +4760,7 @@
       <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.5703125" defaultRowHeight="21.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="22.5703125" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
@@ -4780,7 +4776,7 @@
     <col min="13" max="13" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21.75" customHeight="1">
+    <row r="1" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>178</v>
       </c>
@@ -4827,7 +4823,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="2" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4860,7 +4856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="3" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4892,7 +4888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="4" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4924,7 +4920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="5" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4956,7 +4952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="6" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4988,7 +4984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="7" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5020,7 +5016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="8" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5052,7 +5048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="9" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5084,7 +5080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="10" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5116,7 +5112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="11" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5148,7 +5144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="12" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5180,7 +5176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="13" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5212,7 +5208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="14" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5244,7 +5240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="15" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5276,7 +5272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="16" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5308,7 +5304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="17" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5340,7 +5336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="18" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5372,7 +5368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="19" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5404,7 +5400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="20" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5436,7 +5432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="21" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5468,7 +5464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="22" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5500,7 +5496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="23" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5532,7 +5528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="24" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5564,7 +5560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="25" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5596,7 +5592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="26" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5628,7 +5624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="27" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5660,7 +5656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="21.75" customHeight="1">
+    <row r="28" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5694,7 +5690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="21.75" customHeight="1">
+    <row r="29" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5726,7 +5722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="30" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5758,7 +5754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="31" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5790,7 +5786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="21.75" customHeight="1">
+    <row r="32" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5822,7 +5818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="21.75" customHeight="1">
+    <row r="33" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5854,7 +5850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="21.75" customHeight="1">
+    <row r="34" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5886,7 +5882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="35" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5918,7 +5914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="36" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5950,7 +5946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="37" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5982,7 +5978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="21.75" customHeight="1">
+    <row r="38" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -6014,7 +6010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="39" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -6046,7 +6042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="40" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -6078,7 +6074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="21.75" customHeight="1">
+    <row r="41" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -6110,7 +6106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="21.75" customHeight="1">
+    <row r="42" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -6142,7 +6138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="43" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -6174,7 +6170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="44" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -6206,7 +6202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="45" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -6238,7 +6234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="46" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -6270,7 +6266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="47" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -6302,7 +6298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="48" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -6334,7 +6330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="49" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -6366,7 +6362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="21.75" hidden="1" customHeight="1">
+    <row r="50" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -6398,7 +6394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="21.75" customHeight="1">
+    <row r="51" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -6430,7 +6426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="21.75" customHeight="1">
+    <row r="52" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -6462,7 +6458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="21.75" customHeight="1">
+    <row r="53" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -6517,7 +6513,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6531,7 +6527,7 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.7109375" defaultRowHeight="18.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="19.7109375" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -6545,46 +6541,46 @@
     <col min="12" max="12" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="14" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
+    <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
       <c r="F2" s="9" t="s">
         <v>209</v>
       </c>
@@ -6594,12 +6590,12 @@
       <c r="H2" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-    </row>
-    <row r="3" spans="1:12" ht="18.75" customHeight="1">
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+    </row>
+    <row r="3" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>29</v>
       </c>
@@ -6625,7 +6621,7 @@
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
     </row>
-    <row r="4" spans="1:12" ht="18.75" customHeight="1">
+    <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>65</v>
       </c>
@@ -6651,7 +6647,7 @@
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
     </row>
-    <row r="5" spans="1:12" ht="18.75" customHeight="1">
+    <row r="5" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>111</v>
       </c>
@@ -6677,7 +6673,7 @@
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
     </row>
-    <row r="6" spans="1:12" ht="18.75" customHeight="1">
+    <row r="6" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>176</v>
       </c>
@@ -6705,16 +6701,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6728,12 +6724,12 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.5703125" defaultRowHeight="22.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="22.5703125" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="22.5" customHeight="1" thickBot="1">
+    <row r="1" spans="1:9" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6746,11 +6742,11 @@
       <c r="D1" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
       <c r="H1" s="3" t="s">
         <v>219</v>
       </c>
@@ -6758,7 +6754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="22.5" customHeight="1" thickBot="1">
+    <row r="2" spans="1:9" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -6783,7 +6779,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" ht="22.5" customHeight="1" thickBot="1">
+    <row r="3" spans="1:9" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>64</v>
       </c>
@@ -6802,7 +6798,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="22.5" customHeight="1" thickBot="1">
+    <row r="4" spans="1:9" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>110</v>
       </c>
@@ -6821,7 +6817,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" ht="22.5" customHeight="1" thickBot="1">
+    <row r="5" spans="1:9" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>173</v>
       </c>
@@ -6840,7 +6836,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" ht="22.5" customHeight="1">
+    <row r="6" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>

</xml_diff>

<commit_message>
Convert to GitHub Pages: Read Excel from GitHub, use HashRouter, add deployment scripts
</commit_message>
<xml_diff>
--- a/backend/data/rudraram_survey.xlsx
+++ b/backend/data/rudraram_survey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\OneDrive\Desktop\StartUp\Rudraram Survey\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9D1656-233A-4985-8024-B25F07D41354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560518DA-99B0-48FB-89B2-0481C9694254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -949,14 +949,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1196,7 +1196,7 @@
   <dimension ref="A1:M64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2992,6 +2992,7 @@
     <mergeCell ref="A34:L34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3966,7 +3967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3998,7 +3999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4126,7 +4127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4158,7 +4159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4190,7 +4191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4254,7 +4255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4286,7 +4287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4382,7 +4383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4414,7 +4415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4446,7 +4447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4478,7 +4479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4510,7 +4511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4542,7 +4543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4574,7 +4575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4606,7 +4607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4739,11 +4740,6 @@
     <filterColumn colId="3">
       <filters>
         <filter val="Waddera"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Working"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4756,8 +4752,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.5703125" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5722,7 +5718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5754,7 +5750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5882,7 +5878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5914,7 +5910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5946,7 +5942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -6010,7 +6006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -6042,7 +6038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -6138,7 +6134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -6170,7 +6166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -6202,7 +6198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -6234,7 +6230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -6266,7 +6262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -6298,7 +6294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -6330,7 +6326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -6362,7 +6358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -6495,11 +6491,6 @@
     <filterColumn colId="3">
       <filters>
         <filter val="Waddera"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Working"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -6542,45 +6533,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16" t="s">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="16" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
       <c r="F2" s="9" t="s">
         <v>209</v>
       </c>
@@ -6590,10 +6581,10 @@
       <c r="H2" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
     </row>
     <row r="3" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
@@ -6701,16 +6692,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6742,11 +6733,11 @@
       <c r="D1" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
       <c r="H1" s="3" t="s">
         <v>219</v>
       </c>

</xml_diff>

<commit_message>
Feature: Comprehensive Map UI Enhancement
- Added heatmap/cluster/markers view mode toggle
- Implemented device type filters (Borewell, Sump, OHSR, OHT)
- Created custom status-based icons with color coding:
  * Green for Working devices
  * Red for Non-Working devices
  * Grey for Failed devices
- Increased max zoom from 22x to 30x for detailed inspection
- Added HeatmapLayer component using leaflet.heat
- Created CustomMarkerIcons with SVG-based device type icons
- Improved UI alignment and filter panel organization
- Updated Excel data file with manual changes

All features tested and working seamlessly.
</commit_message>
<xml_diff>
--- a/backend/data/rudraram_survey.xlsx
+++ b/backend/data/rudraram_survey.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\OneDrive\Desktop\StartUp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\OneDrive\Desktop\StartUp\Rudraram Survey\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF0FD0AB-21ED-4352-9F16-4125B365CEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB2CC20-393E-4F95-9F2F-F9F6A79329D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1079,7 +1079,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1103,7 +1103,6 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
@@ -1142,49 +1141,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="55">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF1F1F1F"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1696,29 +1657,65 @@
       </border>
     </dxf>
     <dxf>
-      <border>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF1F1F1F"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF1F1F1F"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2208,6 +2205,41 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF1F1F1F"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -2222,12 +2254,14 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2612,16 +2646,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <top style="thin">
           <color auto="1"/>
-        </bottom>
+        </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
+        <bottom style="thin">
           <color auto="1"/>
-        </top>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2652,44 +2686,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF1F1F1F"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF1F1F1F"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2722,35 +2718,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{417347F4-6754-4B8E-A57B-03D9BD91EBC4}" name="Table1" displayName="Table1" ref="A1:Q61" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="50" tableBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{417347F4-6754-4B8E-A57B-03D9BD91EBC4}" name="Table1" displayName="Table1" ref="A1:Q61" totalsRowShown="0" headerRowDxfId="54" headerRowBorderDxfId="53" tableBorderDxfId="52">
   <autoFilter ref="A1:Q61" xr:uid="{417347F4-6754-4B8E-A57B-03D9BD91EBC4}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{34DFFDD7-E928-49E1-8CE8-BD43990EC130}" name="Sr. No." dataDxfId="49">
+    <tableColumn id="1" xr3:uid="{34DFFDD7-E928-49E1-8CE8-BD43990EC130}" name="Sr. No." dataDxfId="51">
       <calculatedColumnFormula>A1+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C4E25BB6-20A2-440A-98B9-CE8C0738D056}" name="Survey Code (ID)" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{DB53DAC9-0D39-4A5B-B5B8-5B21144AD521}" name="Original Name" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{65C434A5-5189-4A45-9A8A-F4BA84905845}" name="Zone" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{AC05ED28-EFC8-4540-A031-B11F93ABFA84}" name="Location" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{7F01E131-6E29-4CCA-884A-D4FDAA967D9E}" name="Status" dataDxfId="44"/>
-    <tableColumn id="7" xr3:uid="{82E17CC2-8916-4589-8A66-253F0F5AE9A0}" name="Depth (ft)" dataDxfId="43"/>
-    <tableColumn id="8" xr3:uid="{4F1C7970-1F05-4088-B1BB-FDE244B3B894}" name="Motor HP" dataDxfId="42"/>
-    <tableColumn id="9" xr3:uid="{15218248-06B6-4226-9B3D-7C6FBDFCFB75}" name="Pipe Size (inch)" dataDxfId="41"/>
-    <tableColumn id="16" xr3:uid="{D13790CA-5847-4B8D-9699-54C7BBD19736}" name="Latitude" dataDxfId="40"/>
-    <tableColumn id="17" xr3:uid="{F233C6E8-98D0-4A6D-B8F7-60A045108AD0}" name="Longitude" dataDxfId="39"/>
-    <tableColumn id="10" xr3:uid="{D8773AAC-8029-427D-8F0F-92390460C5F3}" name="Houses Connected" dataDxfId="38"/>
-    <tableColumn id="11" xr3:uid="{4A840690-5741-41F2-B477-4C6E191AA29A}" name="Daily Usage (Hrs)" dataDxfId="37"/>
-    <tableColumn id="12" xr3:uid="{94479AD6-BD6F-459E-8BF2-2EFDE558E65C}" name="Power Type (1Ph/3Ph)" dataDxfId="36"/>
-    <tableColumn id="13" xr3:uid="{775457A4-36F4-428A-914B-6F7FF2313CC3}" name="Notes" dataDxfId="35"/>
-    <tableColumn id="14" xr3:uid="{4E1E4528-2F7D-4491-99FB-506D4E73C12C}" name="Images" dataDxfId="34"/>
-    <tableColumn id="15" xr3:uid="{51D1C202-9495-49B1-8EF5-C2839246C8D2}" name="Done" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{C4E25BB6-20A2-440A-98B9-CE8C0738D056}" name="Survey Code (ID)" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{DB53DAC9-0D39-4A5B-B5B8-5B21144AD521}" name="Original Name" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{65C434A5-5189-4A45-9A8A-F4BA84905845}" name="Zone" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{AC05ED28-EFC8-4540-A031-B11F93ABFA84}" name="Location" dataDxfId="47"/>
+    <tableColumn id="6" xr3:uid="{7F01E131-6E29-4CCA-884A-D4FDAA967D9E}" name="Status" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{82E17CC2-8916-4589-8A66-253F0F5AE9A0}" name="Depth (ft)" dataDxfId="45"/>
+    <tableColumn id="8" xr3:uid="{4F1C7970-1F05-4088-B1BB-FDE244B3B894}" name="Motor HP" dataDxfId="44"/>
+    <tableColumn id="9" xr3:uid="{15218248-06B6-4226-9B3D-7C6FBDFCFB75}" name="Pipe Size (inch)" dataDxfId="43"/>
+    <tableColumn id="16" xr3:uid="{D13790CA-5847-4B8D-9699-54C7BBD19736}" name="Latitude" dataDxfId="42"/>
+    <tableColumn id="17" xr3:uid="{F233C6E8-98D0-4A6D-B8F7-60A045108AD0}" name="Longitude" dataDxfId="41"/>
+    <tableColumn id="10" xr3:uid="{D8773AAC-8029-427D-8F0F-92390460C5F3}" name="Houses Connected" dataDxfId="40"/>
+    <tableColumn id="11" xr3:uid="{4A840690-5741-41F2-B477-4C6E191AA29A}" name="Daily Usage (Hrs)" dataDxfId="39"/>
+    <tableColumn id="12" xr3:uid="{94479AD6-BD6F-459E-8BF2-2EFDE558E65C}" name="Power Type (1Ph/3Ph)" dataDxfId="38"/>
+    <tableColumn id="13" xr3:uid="{775457A4-36F4-428A-914B-6F7FF2313CC3}" name="Notes" dataDxfId="37"/>
+    <tableColumn id="14" xr3:uid="{4E1E4528-2F7D-4491-99FB-506D4E73C12C}" name="Images" dataDxfId="36"/>
+    <tableColumn id="15" xr3:uid="{51D1C202-9495-49B1-8EF5-C2839246C8D2}" name="Done" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{92358DA4-6098-4D02-91E8-B3FE4703861C}" name="Table3" displayName="Table3" ref="A1:L5" totalsRowShown="0" headerRowDxfId="17" dataDxfId="53" headerRowBorderDxfId="31" tableBorderDxfId="32" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{92358DA4-6098-4D02-91E8-B3FE4703861C}" name="Table3" displayName="Table3" ref="A1:L5" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="A1:L5" xr:uid="{92358DA4-6098-4D02-91E8-B3FE4703861C}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{3FF01A21-9140-4E7D-B228-830AA3833B90}" name="Survey Code (ID)" dataDxfId="29"/>
@@ -2771,22 +2767,22 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0D993007-6A32-4206-A327-70EC2F57D9AE}" name="Table2" displayName="Table2" ref="A1:M6" totalsRowShown="0" headerRowDxfId="0" dataDxfId="54" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0D993007-6A32-4206-A327-70EC2F57D9AE}" name="Table2" displayName="Table2" ref="A1:M6" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:M6" xr:uid="{0D993007-6A32-4206-A327-70EC2F57D9AE}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{2B6529ED-85DF-41C0-A8F4-8051DCE078C0}" name="Survey Code (ID)" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{2D2A791B-39A9-454A-B1AF-C0D4AADC9452}" name="Original Name" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{2792ED82-9950-4453-AB4F-8A0F3CF4D416}" name="Zone" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{B17B0DFA-985D-4BC2-B67A-CEEC462A0245}" name="Location" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{E4A959AD-D1CA-4D59-9537-EF4ED2AF6D9F}" name="Capacity" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{506764B2-66CB-4967-8355-D96452B14705}" name="Type" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{E07B8A50-88CD-44ED-BC0B-A8377EB93840}" name="Tank Height (m)" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{F63DFB33-0813-4848-8F88-2426E081FF5F}" name="Latitude" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{3D6BE415-29B7-4737-A9D8-F73472C864A1}" name="Longitude" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{ADC7E1B1-C36A-4F6C-952C-8F8166C71D80}" name="Material" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{5B738BA2-2814-4701-A89F-5F63CD6CD798}" name="Lid Access?" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{E0CE272C-DF74-440D-955B-7AE7D2838F68}" name="Houses Connected" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{6966ED3B-E49D-43FA-A1C6-E200DAEE8D0B}" name="Images" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{2B6529ED-85DF-41C0-A8F4-8051DCE078C0}" name="Survey Code (ID)" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{2D2A791B-39A9-454A-B1AF-C0D4AADC9452}" name="Original Name" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{2792ED82-9950-4453-AB4F-8A0F3CF4D416}" name="Zone" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{B17B0DFA-985D-4BC2-B67A-CEEC462A0245}" name="Location" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{E4A959AD-D1CA-4D59-9537-EF4ED2AF6D9F}" name="Capacity" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{506764B2-66CB-4967-8355-D96452B14705}" name="Type" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{E07B8A50-88CD-44ED-BC0B-A8377EB93840}" name="Tank Height (m)" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{F63DFB33-0813-4848-8F88-2426E081FF5F}" name="Latitude" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{3D6BE415-29B7-4737-A9D8-F73472C864A1}" name="Longitude" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{ADC7E1B1-C36A-4F6C-952C-8F8166C71D80}" name="Material" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{5B738BA2-2814-4701-A89F-5F63CD6CD798}" name="Lid Access?" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{E0CE272C-DF74-440D-955B-7AE7D2838F68}" name="Houses Connected" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{6966ED3B-E49D-43FA-A1C6-E200DAEE8D0B}" name="Images" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3082,7 +3078,7 @@
   <dimension ref="A1:Q61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="43" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3188,10 +3184,10 @@
         <v>73</v>
       </c>
       <c r="J2" s="6">
-        <v>17.55336746</v>
+        <v>17.55335226</v>
       </c>
       <c r="K2" s="6">
-        <v>78.334846999999996</v>
+        <v>78.163334144999993</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
@@ -3368,7 +3364,7 @@
       <c r="H6" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="6">
         <v>1</v>
       </c>
       <c r="J6" s="6">
@@ -3687,7 +3683,7 @@
       <c r="H13" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="6">
         <v>2</v>
       </c>
       <c r="J13" s="6">
@@ -3781,7 +3777,7 @@
       <c r="H15" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="6">
         <v>1.5</v>
       </c>
       <c r="J15" s="6">
@@ -3828,7 +3824,7 @@
       <c r="H16" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="6">
         <v>1</v>
       </c>
       <c r="J16" s="6">
@@ -3967,7 +3963,7 @@
       <c r="H19" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="6">
         <v>1</v>
       </c>
       <c r="J19" s="6">
@@ -4153,7 +4149,7 @@
       <c r="H23" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I23" s="6">
         <v>1</v>
       </c>
       <c r="J23" s="6">
@@ -4198,7 +4194,7 @@
       <c r="H24" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I24" s="6">
         <v>1</v>
       </c>
       <c r="J24" s="6">
@@ -4265,7 +4261,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
-        <f>A25+1</f>
+        <f t="shared" ref="A26:A61" si="0">A25+1</f>
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -4313,7 +4309,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
-        <f>A26+1</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
@@ -4361,7 +4357,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
-        <f>A27+1</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
@@ -4407,7 +4403,7 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
-        <f>A28+1</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
@@ -4455,7 +4451,7 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
-        <f>A29+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
@@ -4503,7 +4499,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
-        <f>A30+1</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
@@ -4549,7 +4545,7 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
-        <f>A31+1</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
@@ -4597,7 +4593,7 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
-        <f>A32+1</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
@@ -4645,7 +4641,7 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
-        <f>A33+1</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
@@ -4691,7 +4687,7 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
-        <f>A34+1</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
@@ -4739,7 +4735,7 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
-        <f>A35+1</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
@@ -4785,7 +4781,7 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
-        <f>A36+1</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
@@ -4833,7 +4829,7 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
-        <f>A37+1</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
@@ -4881,7 +4877,7 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
-        <f>A38+1</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
@@ -4929,7 +4925,7 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
-        <f>A39+1</f>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -4975,7 +4971,7 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
-        <f>A40+1</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
@@ -5023,7 +5019,7 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
-        <f>A41+1</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
@@ -5069,7 +5065,7 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
-        <f>A42+1</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="B43" s="6" t="s">
@@ -5115,7 +5111,7 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
-        <f>A43+1</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="B44" s="6" t="s">
@@ -5161,7 +5157,7 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
-        <f>A44+1</f>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="B45" s="6" t="s">
@@ -5209,7 +5205,7 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
-        <f>A45+1</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="B46" s="6" t="s">
@@ -5257,7 +5253,7 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
-        <f>A46+1</f>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -5305,7 +5301,7 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
-        <f>A47+1</f>
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="B48" s="6" t="s">
@@ -5353,7 +5349,7 @@
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
-        <f>A48+1</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="B49" s="6" t="s">
@@ -5399,7 +5395,7 @@
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
-        <f>A49+1</f>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="B50" s="6" t="s">
@@ -5447,7 +5443,7 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
-        <f>A50+1</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -5485,7 +5481,7 @@
       <c r="N51" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="O51" s="10" t="s">
+      <c r="O51" s="9" t="s">
         <v>229</v>
       </c>
       <c r="P51" s="6"/>
@@ -5495,7 +5491,7 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
-        <f>A51+1</f>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="B52" s="6" t="s">
@@ -5541,7 +5537,7 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
-        <f>A52+1</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="B53" s="6" t="s">
@@ -5587,7 +5583,7 @@
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
-        <f>A53+1</f>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="B54" s="6" t="s">
@@ -5633,7 +5629,7 @@
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
-        <f>A54+1</f>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="B55" s="6" t="s">
@@ -5679,7 +5675,7 @@
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
-        <f>A55+1</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="B56" s="6" t="s">
@@ -5727,7 +5723,7 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
-        <f>A56+1</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -5775,7 +5771,7 @@
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
-        <f>A57+1</f>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="B58" s="6" t="s">
@@ -5823,7 +5819,7 @@
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
-        <f>A58+1</f>
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="B59" s="6" t="s">
@@ -5869,7 +5865,7 @@
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
-        <f>A59+1</f>
+        <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="B60" s="6" t="s">
@@ -5915,7 +5911,7 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
-        <f>A60+1</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="B61" s="6" t="s">
@@ -5993,40 +5989,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -6058,7 +6054,7 @@
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="15"/>
+      <c r="L2" s="14"/>
     </row>
     <row r="3" spans="1:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -6088,7 +6084,7 @@
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
-      <c r="L3" s="15"/>
+      <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -6118,37 +6114,37 @@
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="15"/>
+      <c r="L4" s="14"/>
     </row>
     <row r="5" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>249</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17">
+      <c r="G5" s="16"/>
+      <c r="H5" s="16">
         <v>17.554371549999999</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="16">
         <v>78.163831639999998</v>
       </c>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="18"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6182,43 +6178,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>243</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="20" t="s">
         <v>12</v>
       </c>
     </row>
@@ -6253,7 +6249,7 @@
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="15"/>
+      <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -6286,7 +6282,7 @@
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="15"/>
+      <c r="M3" s="14"/>
     </row>
     <row r="4" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -6319,7 +6315,7 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="15"/>
+      <c r="M4" s="14"/>
     </row>
     <row r="5" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -6352,39 +6348,39 @@
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="15"/>
+      <c r="M5" s="14"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>275</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>280</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>249</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>268</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="24">
+      <c r="G6" s="22"/>
+      <c r="H6" s="16">
         <v>17.554403279999999</v>
       </c>
-      <c r="I6" s="24">
+      <c r="I6" s="16">
         <v>78.163868460000003</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
       <c r="M6" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Map visibility, Custom Icons, Zone Filter, and Sump/OHSR status
1. Fixed Map Visibility by ensuring CSS height is 100%. 2. Updated CustomMarkerIcons to use Circle(Borewell), Box(Sump), Box/O(OHSR) with requested colors. 3. Filtered Zones page to only Waddera Colony, Village, SC Colony. 4. Forced 'Working' status for Sump/OHSR in backend.
</commit_message>
<xml_diff>
--- a/backend/data/rudraram_survey.xlsx
+++ b/backend/data/rudraram_survey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\OneDrive\Desktop\StartUp\Rudraram Survey\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB2CC20-393E-4F95-9F2F-F9F6A79329D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B745311E-F61A-4B73-A34F-314D97982B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="282">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -785,9 +785,6 @@
   </si>
   <si>
     <t>Mandal Parishad School</t>
-  </si>
-  <si>
-    <t>Waddera</t>
   </si>
   <si>
     <t>Water Work Yard</t>
@@ -3077,8 +3074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="43" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="123" zoomScaleNormal="43" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3131,10 +3128,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>9</v>
@@ -5971,21 +5968,23 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
-    <col min="8" max="9" width="21.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6008,19 +6007,19 @@
         <v>247</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>281</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>282</v>
       </c>
       <c r="J1" s="11" t="s">
         <v>244</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>12</v>
@@ -6028,10 +6027,10 @@
     </row>
     <row r="2" spans="1:12" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>199</v>
@@ -6043,7 +6042,7 @@
         <v>246</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2">
@@ -6058,10 +6057,10 @@
     </row>
     <row r="3" spans="1:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>151</v>
@@ -6073,7 +6072,7 @@
         <v>246</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3">
@@ -6088,22 +6087,22 @@
     </row>
     <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>250</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>246</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3">
@@ -6118,22 +6117,22 @@
     </row>
     <row r="5" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C5" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>249</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>250</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>246</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G5" s="16"/>
       <c r="H5" s="16">
@@ -6160,21 +6159,24 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="9" width="16.85546875" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6194,22 +6196,22 @@
         <v>243</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>247</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="I1" s="12" t="s">
-        <v>282</v>
-      </c>
       <c r="J1" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="K1" s="19" t="s">
         <v>264</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>265</v>
       </c>
       <c r="L1" s="19" t="s">
         <v>9</v>
@@ -6220,10 +6222,10 @@
     </row>
     <row r="2" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>199</v>
@@ -6235,7 +6237,7 @@
         <v>246</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3">
@@ -6245,7 +6247,7 @@
         <v>78.169125199999996</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -6253,10 +6255,10 @@
     </row>
     <row r="3" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>151</v>
@@ -6265,10 +6267,10 @@
         <v>248</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3">
@@ -6278,7 +6280,7 @@
         <v>78.165223179999998</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -6286,10 +6288,10 @@
     </row>
     <row r="4" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>151</v>
@@ -6298,10 +6300,10 @@
         <v>248</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3">
@@ -6311,7 +6313,7 @@
         <v>78.165299050000002</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -6319,22 +6321,22 @@
     </row>
     <row r="5" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>249</v>
+        <v>37</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>245</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3">
@@ -6344,30 +6346,30 @@
         <v>78.163861549999993</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="14"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>249</v>
+        <v>37</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>245</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="16">
@@ -6377,7 +6379,7 @@
         <v>78.163868460000003</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K6" s="22"/>
       <c r="L6" s="22"/>

</xml_diff>